<commit_message>
Apply is_word check to lexical density and lexical diversity
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/news_and_blog/Fakespeak_news_and_blog_lexical_density.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/news_and_blog/Fakespeak_news_and_blog_lexical_density.xlsx
@@ -1851,7 +1851,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.4594594594594595</v>
+        <v>0.53125</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1859,7 +1859,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.3931203931203931</v>
+        <v>0.4678362573099415</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1867,7 +1867,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.5930735930735931</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1875,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.5413223140495868</v>
+        <v>0.6150234741784038</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1883,7 +1883,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.4622950819672131</v>
+        <v>0.546875</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1891,7 +1891,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.486318407960199</v>
+        <v>0.5534950071326676</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1899,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.4744318181818182</v>
+        <v>0.5369774919614148</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1907,7 +1907,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.5473684210526316</v>
+        <v>0.6216216216216216</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1915,7 +1915,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.480565371024735</v>
+        <v>0.5461847389558233</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1923,7 +1923,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.5413375460768826</v>
+        <v>0.6168674698795181</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1931,7 +1931,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.4532710280373832</v>
+        <v>0.512549537648613</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1939,7 +1939,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.4865671641791044</v>
+        <v>0.5790408525754884</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1947,7 +1947,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.4430072756669362</v>
+        <v>0.5126522961574508</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1955,7 +1955,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.5608974358974359</v>
+        <v>0.6225402504472272</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1963,7 +1963,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.515878616796048</v>
+        <v>0.5852090032154341</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1971,7 +1971,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.4525547445255474</v>
+        <v>0.5346964064436184</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1979,7 +1979,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.4238227146814404</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1987,7 +1987,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.4458204334365325</v>
+        <v>0.5239852398523985</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1995,7 +1995,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.4634146341463415</v>
+        <v>0.5205479452054794</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2024,7 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.5857142857142857</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2032,7 +2032,7 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>0.5161290322580645</v>
+        <v>0.587037037037037</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2040,7 +2040,7 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>0.5317848410757946</v>
+        <v>0.6251203079884504</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2048,7 +2048,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>0.4473684210526316</v>
+        <v>0.4857142857142857</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2056,7 +2056,7 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>0.4735729386892177</v>
+        <v>0.5544554455445545</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2064,7 +2064,7 @@
         <v>26</v>
       </c>
       <c r="B7">
-        <v>0.4390893678856866</v>
+        <v>0.5395446375074895</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2072,7 +2072,7 @@
         <v>27</v>
       </c>
       <c r="B8">
-        <v>0.4868210862619808</v>
+        <v>0.56209453197405</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2080,7 +2080,7 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <v>0.5093167701863354</v>
+        <v>0.568445475638051</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2088,7 +2088,7 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>0.6702127659574468</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2096,7 +2096,7 @@
         <v>30</v>
       </c>
       <c r="B11">
-        <v>0.5189075630252101</v>
+        <v>0.6049382716049383</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2104,7 +2104,7 @@
         <v>31</v>
       </c>
       <c r="B12">
-        <v>0.4630681818181818</v>
+        <v>0.530278232405892</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2112,7 +2112,7 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>0.5095541401273885</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2120,7 +2120,7 @@
         <v>33</v>
       </c>
       <c r="B14">
-        <v>0.4360655737704918</v>
+        <v>0.5175097276264592</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2128,7 +2128,7 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>0.4794188861985472</v>
+        <v>0.559322033898305</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2136,7 +2136,7 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>0.4944488501189532</v>
+        <v>0.5767981438515081</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2144,7 +2144,7 @@
         <v>36</v>
       </c>
       <c r="B17">
-        <v>0.4807017543859649</v>
+        <v>0.545816733067729</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2152,7 +2152,7 @@
         <v>37</v>
       </c>
       <c r="B18">
-        <v>0.4406779661016949</v>
+        <v>0.5131578947368421</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2160,7 +2160,7 @@
         <v>38</v>
       </c>
       <c r="B19">
-        <v>0.5287958115183246</v>
+        <v>0.5894428152492669</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2168,7 +2168,7 @@
         <v>39</v>
       </c>
       <c r="B20">
-        <v>0.4606824925816024</v>
+        <v>0.5506216696269982</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2176,7 +2176,7 @@
         <v>40</v>
       </c>
       <c r="B21">
-        <v>0.4712990936555891</v>
+        <v>0.5342465753424658</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2184,7 +2184,7 @@
         <v>41</v>
       </c>
       <c r="B22">
-        <v>0.4918918918918919</v>
+        <v>0.5723270440251572</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2192,7 +2192,7 @@
         <v>42</v>
       </c>
       <c r="B23">
-        <v>0.4756756756756757</v>
+        <v>0.5598705501618123</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2200,7 +2200,7 @@
         <v>43</v>
       </c>
       <c r="B24">
-        <v>0.5138888888888888</v>
+        <v>0.6123595505617978</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2208,7 +2208,7 @@
         <v>44</v>
       </c>
       <c r="B25">
-        <v>0.4750733137829912</v>
+        <v>0.5806451612903226</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2216,7 +2216,7 @@
         <v>45</v>
       </c>
       <c r="B26">
-        <v>0.4636752136752137</v>
+        <v>0.5725593667546174</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2224,7 +2224,7 @@
         <v>46</v>
       </c>
       <c r="B27">
-        <v>0.5160744500846024</v>
+        <v>0.6244813278008299</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2232,7 +2232,7 @@
         <v>47</v>
       </c>
       <c r="B28">
-        <v>0.5492227979274611</v>
+        <v>0.695364238410596</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2240,7 +2240,7 @@
         <v>48</v>
       </c>
       <c r="B29">
-        <v>0.46875</v>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2248,7 +2248,7 @@
         <v>49</v>
       </c>
       <c r="B30">
-        <v>0.4742217898832685</v>
+        <v>0.5248380129589633</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2256,7 +2256,7 @@
         <v>50</v>
       </c>
       <c r="B31">
-        <v>0.4909847434119279</v>
+        <v>0.5784313725490197</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2264,7 +2264,7 @@
         <v>51</v>
       </c>
       <c r="B32">
-        <v>0.4463869463869464</v>
+        <v>0.518796992481203</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2272,7 +2272,7 @@
         <v>52</v>
       </c>
       <c r="B33">
-        <v>0.4752136752136752</v>
+        <v>0.5618661257606491</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2280,7 +2280,7 @@
         <v>53</v>
       </c>
       <c r="B34">
-        <v>0.4619164619164619</v>
+        <v>0.5164835164835165</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2288,7 +2288,7 @@
         <v>54</v>
       </c>
       <c r="B35">
-        <v>0.468677494199536</v>
+        <v>0.5422343324250681</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2296,7 +2296,7 @@
         <v>55</v>
       </c>
       <c r="B36">
-        <v>0.4070021881838075</v>
+        <v>0.4757033248081842</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2304,7 +2304,7 @@
         <v>56</v>
       </c>
       <c r="B37">
-        <v>0.4678111587982833</v>
+        <v>0.5343137254901961</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2312,7 +2312,7 @@
         <v>57</v>
       </c>
       <c r="B38">
-        <v>0.5303643724696356</v>
+        <v>0.6632653061224489</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -2320,7 +2320,7 @@
         <v>58</v>
       </c>
       <c r="B39">
-        <v>0.4559471365638766</v>
+        <v>0.5269922879177378</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -2328,7 +2328,7 @@
         <v>59</v>
       </c>
       <c r="B40">
-        <v>0.4567901234567901</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -2336,7 +2336,7 @@
         <v>60</v>
       </c>
       <c r="B41">
-        <v>0.4635416666666667</v>
+        <v>0.5465838509316771</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2344,7 +2344,7 @@
         <v>61</v>
       </c>
       <c r="B42">
-        <v>0.4656549520766773</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2352,7 +2352,7 @@
         <v>62</v>
       </c>
       <c r="B43">
-        <v>0.6035829122645843</v>
+        <v>0.6874508776526067</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2360,7 +2360,7 @@
         <v>63</v>
       </c>
       <c r="B44">
-        <v>0.5385694249649369</v>
+        <v>0.5990491283676703</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2368,7 +2368,7 @@
         <v>64</v>
       </c>
       <c r="B45">
-        <v>0.5127478753541076</v>
+        <v>0.5868852459016394</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2376,7 +2376,7 @@
         <v>65</v>
       </c>
       <c r="B46">
-        <v>0.4739336492890995</v>
+        <v>0.5602240896358543</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2384,7 +2384,7 @@
         <v>66</v>
       </c>
       <c r="B47">
-        <v>0.453427065026362</v>
+        <v>0.5286885245901639</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2392,7 +2392,7 @@
         <v>67</v>
       </c>
       <c r="B48">
-        <v>0.4723618090452261</v>
+        <v>0.5578635014836796</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2400,7 +2400,7 @@
         <v>68</v>
       </c>
       <c r="B49">
-        <v>0.462478184991274</v>
+        <v>0.5398773006134969</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2408,7 +2408,7 @@
         <v>69</v>
       </c>
       <c r="B50">
-        <v>0.4481074481074481</v>
+        <v>0.5328467153284672</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2416,7 +2416,7 @@
         <v>70</v>
       </c>
       <c r="B51">
-        <v>0.4562383612662942</v>
+        <v>0.5185577942735949</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2424,7 +2424,7 @@
         <v>71</v>
       </c>
       <c r="B52">
-        <v>0.4303448275862069</v>
+        <v>0.5157545605306799</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2432,7 +2432,7 @@
         <v>72</v>
       </c>
       <c r="B53">
-        <v>0.4518072289156627</v>
+        <v>0.5514705882352942</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2440,7 +2440,7 @@
         <v>73</v>
       </c>
       <c r="B54">
-        <v>0.4945355191256831</v>
+        <v>0.5764331210191083</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2448,7 +2448,7 @@
         <v>74</v>
       </c>
       <c r="B55">
-        <v>0.5513513513513514</v>
+        <v>0.6415094339622641</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2456,7 +2456,7 @@
         <v>75</v>
       </c>
       <c r="B56">
-        <v>0.4651162790697674</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2464,7 +2464,7 @@
         <v>76</v>
       </c>
       <c r="B57">
-        <v>0.5457516339869281</v>
+        <v>0.6117216117216118</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2472,7 +2472,7 @@
         <v>77</v>
       </c>
       <c r="B58">
-        <v>0.5652173913043478</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2480,7 +2480,7 @@
         <v>78</v>
       </c>
       <c r="B59">
-        <v>0.5209205020920502</v>
+        <v>0.5971223021582733</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2488,7 +2488,7 @@
         <v>79</v>
       </c>
       <c r="B60">
-        <v>0.4916773367477593</v>
+        <v>0.5626865671641791</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2496,7 +2496,7 @@
         <v>80</v>
       </c>
       <c r="B61">
-        <v>0.5197313182199832</v>
+        <v>0.6143856143856143</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2504,7 +2504,7 @@
         <v>81</v>
       </c>
       <c r="B62">
-        <v>0.4817610062893082</v>
+        <v>0.5661218424962853</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2512,7 +2512,7 @@
         <v>82</v>
       </c>
       <c r="B63">
-        <v>0.4866310160427808</v>
+        <v>0.5476673427991886</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2520,7 +2520,7 @@
         <v>83</v>
       </c>
       <c r="B64">
-        <v>0.4877126654064272</v>
+        <v>0.5491452991452992</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2528,7 +2528,7 @@
         <v>84</v>
       </c>
       <c r="B65">
-        <v>0.4368131868131868</v>
+        <v>0.5071770334928229</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2536,7 +2536,7 @@
         <v>85</v>
       </c>
       <c r="B66">
-        <v>0.4405405405405405</v>
+        <v>0.5344262295081967</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2544,7 +2544,7 @@
         <v>86</v>
       </c>
       <c r="B67">
-        <v>0.4694835680751174</v>
+        <v>0.5620300751879699</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2552,7 +2552,7 @@
         <v>87</v>
       </c>
       <c r="B68">
-        <v>0.4309859154929577</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2560,7 +2560,7 @@
         <v>88</v>
       </c>
       <c r="B69">
-        <v>0.4763313609467456</v>
+        <v>0.544839255499154</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2568,7 +2568,7 @@
         <v>89</v>
       </c>
       <c r="B70">
-        <v>0.5260223048327137</v>
+        <v>0.5915789473684211</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2576,7 +2576,7 @@
         <v>90</v>
       </c>
       <c r="B71">
-        <v>0.510351966873706</v>
+        <v>0.5850178359096314</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2584,7 +2584,7 @@
         <v>91</v>
       </c>
       <c r="B72">
-        <v>0.4348118279569892</v>
+        <v>0.5282093213409649</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2592,7 +2592,7 @@
         <v>92</v>
       </c>
       <c r="B73">
-        <v>0.4947368421052631</v>
+        <v>0.551433389544688</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2600,7 +2600,7 @@
         <v>93</v>
       </c>
       <c r="B74">
-        <v>0.4439071566731141</v>
+        <v>0.5324825986078886</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2608,7 +2608,7 @@
         <v>94</v>
       </c>
       <c r="B75">
-        <v>0.5032119914346895</v>
+        <v>0.59846547314578</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2616,7 +2616,7 @@
         <v>95</v>
       </c>
       <c r="B76">
-        <v>0.4746835443037974</v>
+        <v>0.5826771653543307</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2624,7 +2624,7 @@
         <v>96</v>
       </c>
       <c r="B77">
-        <v>0.4663951120162933</v>
+        <v>0.5682382133995038</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2632,7 +2632,7 @@
         <v>97</v>
       </c>
       <c r="B78">
-        <v>0.5147058823529411</v>
+        <v>0.6091703056768559</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2640,7 +2640,7 @@
         <v>98</v>
       </c>
       <c r="B79">
-        <v>0.5089605734767025</v>
+        <v>0.5916666666666667</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2648,7 +2648,7 @@
         <v>99</v>
       </c>
       <c r="B80">
-        <v>0.4972972972972973</v>
+        <v>0.5939524838012959</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2656,7 +2656,7 @@
         <v>100</v>
       </c>
       <c r="B81">
-        <v>0.4958123953098827</v>
+        <v>0.588469184890656</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2664,7 +2664,7 @@
         <v>101</v>
       </c>
       <c r="B82">
-        <v>0.4614003590664273</v>
+        <v>0.5255623721881391</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2672,7 +2672,7 @@
         <v>102</v>
       </c>
       <c r="B83">
-        <v>0.4133949191685912</v>
+        <v>0.4698162729658792</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2680,7 +2680,7 @@
         <v>103</v>
       </c>
       <c r="B84">
-        <v>0.4361702127659575</v>
+        <v>0.5189873417721519</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2688,7 +2688,7 @@
         <v>104</v>
       </c>
       <c r="B85">
-        <v>0.5284552845528455</v>
+        <v>0.6190476190476191</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2696,7 +2696,7 @@
         <v>105</v>
       </c>
       <c r="B86">
-        <v>0.4784172661870504</v>
+        <v>0.5495867768595041</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2704,7 +2704,7 @@
         <v>106</v>
       </c>
       <c r="B87">
-        <v>0.4803149606299212</v>
+        <v>0.5700934579439252</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2712,7 +2712,7 @@
         <v>107</v>
       </c>
       <c r="B88">
-        <v>0.5448717948717948</v>
+        <v>0.6131386861313869</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2720,7 +2720,7 @@
         <v>108</v>
       </c>
       <c r="B89">
-        <v>0.4408602150537634</v>
+        <v>0.4984709480122324</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2728,7 +2728,7 @@
         <v>109</v>
       </c>
       <c r="B90">
-        <v>0.4656679151061174</v>
+        <v>0.5450516986706057</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2736,7 +2736,7 @@
         <v>110</v>
       </c>
       <c r="B91">
-        <v>0.4642857142857143</v>
+        <v>0.5064935064935064</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2744,7 +2744,7 @@
         <v>111</v>
       </c>
       <c r="B92">
-        <v>0.4636363636363636</v>
+        <v>0.5066666666666667</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2752,7 +2752,7 @@
         <v>112</v>
       </c>
       <c r="B93">
-        <v>0.515625</v>
+        <v>0.5892857142857143</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2760,7 +2760,7 @@
         <v>113</v>
       </c>
       <c r="B94">
-        <v>0.4884792626728111</v>
+        <v>0.5549738219895288</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2768,7 +2768,7 @@
         <v>114</v>
       </c>
       <c r="B95">
-        <v>0.5299145299145299</v>
+        <v>0.6078431372549019</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2776,7 +2776,7 @@
         <v>115</v>
       </c>
       <c r="B96">
-        <v>0.5606936416184971</v>
+        <v>0.6554054054054054</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2784,7 +2784,7 @@
         <v>116</v>
       </c>
       <c r="B97">
-        <v>0.477832512315271</v>
+        <v>0.543661971830986</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2792,7 +2792,7 @@
         <v>117</v>
       </c>
       <c r="B98">
-        <v>0.4201030927835052</v>
+        <v>0.4794117647058824</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2800,7 +2800,7 @@
         <v>118</v>
       </c>
       <c r="B99">
-        <v>0.4455592716462282</v>
+        <v>0.5348627980206928</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2808,7 +2808,7 @@
         <v>119</v>
       </c>
       <c r="B100">
-        <v>0.4343065693430657</v>
+        <v>0.4958333333333333</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2816,7 +2816,7 @@
         <v>120</v>
       </c>
       <c r="B101">
-        <v>0.4933920704845815</v>
+        <v>0.5773195876288659</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2824,7 +2824,7 @@
         <v>121</v>
       </c>
       <c r="B102">
-        <v>0.4839924670433145</v>
+        <v>0.5601750547045952</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2832,7 +2832,7 @@
         <v>122</v>
       </c>
       <c r="B103">
-        <v>0.5268817204301075</v>
+        <v>0.6125</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2840,7 +2840,7 @@
         <v>123</v>
       </c>
       <c r="B104">
-        <v>0.4831181727904668</v>
+        <v>0.5487735310895607</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2848,7 +2848,7 @@
         <v>124</v>
       </c>
       <c r="B105">
-        <v>0.4438775510204082</v>
+        <v>0.5209580838323353</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2856,7 +2856,7 @@
         <v>125</v>
       </c>
       <c r="B106">
-        <v>0.5348837209302325</v>
+        <v>0.6066666666666667</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2864,7 +2864,7 @@
         <v>126</v>
       </c>
       <c r="B107">
-        <v>0.5255712731229597</v>
+        <v>0.5992532669570628</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2872,7 +2872,7 @@
         <v>127</v>
       </c>
       <c r="B108">
-        <v>0.4846625766871165</v>
+        <v>0.5569395017793595</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2880,7 +2880,7 @@
         <v>128</v>
       </c>
       <c r="B109">
-        <v>0.5195729537366548</v>
+        <v>0.5967078189300411</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2888,7 +2888,7 @@
         <v>129</v>
       </c>
       <c r="B110">
-        <v>0.4824902723735409</v>
+        <v>0.5610859728506787</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2896,7 +2896,7 @@
         <v>130</v>
       </c>
       <c r="B111">
-        <v>0.4827586206896552</v>
+        <v>0.5793103448275863</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2904,7 +2904,7 @@
         <v>131</v>
       </c>
       <c r="B112">
-        <v>0.4586466165413534</v>
+        <v>0.5401785714285714</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2912,7 +2912,7 @@
         <v>132</v>
       </c>
       <c r="B113">
-        <v>0.444141689373297</v>
+        <v>0.5126582278481012</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2920,7 +2920,7 @@
         <v>133</v>
       </c>
       <c r="B114">
-        <v>0.4512635379061372</v>
+        <v>0.5535714285714286</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +2949,7 @@
         <v>134</v>
       </c>
       <c r="B2">
-        <v>0.4029850746268657</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2957,7 +2957,7 @@
         <v>135</v>
       </c>
       <c r="B3">
-        <v>0.4760994263862333</v>
+        <v>0.5817757009345794</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2965,7 +2965,7 @@
         <v>136</v>
       </c>
       <c r="B4">
-        <v>0.5081967213114754</v>
+        <v>0.5904761904761905</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2973,7 +2973,7 @@
         <v>137</v>
       </c>
       <c r="B5">
-        <v>0.4867762687634024</v>
+        <v>0.5681818181818182</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2981,7 +2981,7 @@
         <v>138</v>
       </c>
       <c r="B6">
-        <v>0.465818759936407</v>
+        <v>0.5359116022099447</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2989,7 +2989,7 @@
         <v>139</v>
       </c>
       <c r="B7">
-        <v>0.4685230024213075</v>
+        <v>0.5484330484330484</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2997,7 +2997,7 @@
         <v>140</v>
       </c>
       <c r="B8">
-        <v>0.5226738327175008</v>
+        <v>0.6069886140557519</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3005,7 +3005,7 @@
         <v>141</v>
       </c>
       <c r="B9">
-        <v>0.464987714987715</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3013,7 +3013,7 @@
         <v>142</v>
       </c>
       <c r="B10">
-        <v>0.489432703003337</v>
+        <v>0.5446428571428571</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3021,7 +3021,7 @@
         <v>143</v>
       </c>
       <c r="B11">
-        <v>0.4857768052516411</v>
+        <v>0.5558343789209536</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3029,7 +3029,7 @@
         <v>144</v>
       </c>
       <c r="B12">
-        <v>0.449358059914408</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3037,7 +3037,7 @@
         <v>145</v>
       </c>
       <c r="B13">
-        <v>0.455988455988456</v>
+        <v>0.5258764607679466</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3045,7 +3045,7 @@
         <v>146</v>
       </c>
       <c r="B14">
-        <v>0.5289855072463768</v>
+        <v>0.6083333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3053,7 +3053,7 @@
         <v>147</v>
       </c>
       <c r="B15">
-        <v>0.4883720930232558</v>
+        <v>0.5727272727272728</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3061,7 +3061,7 @@
         <v>148</v>
       </c>
       <c r="B16">
-        <v>0.484375</v>
+        <v>0.5568862275449101</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3069,7 +3069,7 @@
         <v>149</v>
       </c>
       <c r="B17">
-        <v>0.5125984251968504</v>
+        <v>0.5855855855855856</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3077,7 +3077,7 @@
         <v>150</v>
       </c>
       <c r="B18">
-        <v>0.5134474327628362</v>
+        <v>0.5867537313432836</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3085,7 +3085,7 @@
         <v>151</v>
       </c>
       <c r="B19">
-        <v>0.4505494505494506</v>
+        <v>0.5051334702258727</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3093,7 +3093,7 @@
         <v>152</v>
       </c>
       <c r="B20">
-        <v>0.4944178628389155</v>
+        <v>0.5764925373134329</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3101,7 +3101,7 @@
         <v>153</v>
       </c>
       <c r="B21">
-        <v>0.5336927223719676</v>
+        <v>0.5863095238095238</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3109,7 +3109,7 @@
         <v>154</v>
       </c>
       <c r="B22">
-        <v>0.4736842105263158</v>
+        <v>0.5316946959896507</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3117,7 +3117,7 @@
         <v>155</v>
       </c>
       <c r="B23">
-        <v>0.4917582417582417</v>
+        <v>0.6310223266745005</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3125,7 +3125,7 @@
         <v>156</v>
       </c>
       <c r="B24">
-        <v>0.4377510040160643</v>
+        <v>0.5142857142857142</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3133,7 +3133,7 @@
         <v>157</v>
       </c>
       <c r="B25">
-        <v>0.4595121951219512</v>
+        <v>0.5237556561085973</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3141,7 +3141,7 @@
         <v>158</v>
       </c>
       <c r="B26">
-        <v>0.5072697899838449</v>
+        <v>0.5954198473282443</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3149,7 +3149,7 @@
         <v>159</v>
       </c>
       <c r="B27">
-        <v>0.4357798165137615</v>
+        <v>0.5205479452054794</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3157,7 +3157,7 @@
         <v>160</v>
       </c>
       <c r="B28">
-        <v>0.4354838709677419</v>
+        <v>0.5242718446601942</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3165,7 +3165,7 @@
         <v>161</v>
       </c>
       <c r="B29">
-        <v>0.5477792732166891</v>
+        <v>0.6277258566978193</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3173,7 +3173,7 @@
         <v>162</v>
       </c>
       <c r="B30">
-        <v>0.4473684210526316</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3181,7 +3181,7 @@
         <v>163</v>
       </c>
       <c r="B31">
-        <v>0.4922600619195047</v>
+        <v>0.5531135531135531</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3189,7 +3189,7 @@
         <v>164</v>
       </c>
       <c r="B32">
-        <v>0.4850835322195704</v>
+        <v>0.5846042120551924</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3197,7 +3197,7 @@
         <v>165</v>
       </c>
       <c r="B33">
-        <v>0.4354207436399217</v>
+        <v>0.5138888888888888</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3205,7 +3205,7 @@
         <v>166</v>
       </c>
       <c r="B34">
-        <v>0.4814814814814815</v>
+        <v>0.5735294117647058</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3213,7 +3213,7 @@
         <v>167</v>
       </c>
       <c r="B35">
-        <v>0.4746031746031746</v>
+        <v>0.5483271375464684</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3221,7 +3221,7 @@
         <v>168</v>
       </c>
       <c r="B36">
-        <v>0.5049900199600799</v>
+        <v>0.6191646191646192</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3229,7 +3229,7 @@
         <v>169</v>
       </c>
       <c r="B37">
-        <v>0.5014245014245015</v>
+        <v>0.5840266222961731</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3237,7 +3237,7 @@
         <v>170</v>
       </c>
       <c r="B38">
-        <v>0.4625267665952891</v>
+        <v>0.5429292929292929</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3245,7 +3245,7 @@
         <v>171</v>
       </c>
       <c r="B39">
-        <v>0.4634831460674158</v>
+        <v>0.5228758169934641</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3253,7 +3253,7 @@
         <v>172</v>
       </c>
       <c r="B40">
-        <v>0.4175824175824176</v>
+        <v>0.4534534534534534</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3261,7 +3261,7 @@
         <v>173</v>
       </c>
       <c r="B41">
-        <v>0.5302279484638256</v>
+        <v>0.5885588558855885</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3269,7 +3269,7 @@
         <v>174</v>
       </c>
       <c r="B42">
-        <v>0.4625228519195612</v>
+        <v>0.5170212765957447</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3277,7 +3277,7 @@
         <v>175</v>
       </c>
       <c r="B43">
-        <v>0.452914798206278</v>
+        <v>0.5410714285714285</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3285,7 +3285,7 @@
         <v>176</v>
       </c>
       <c r="B44">
-        <v>0.4485488126649076</v>
+        <v>0.5329153605015674</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3293,7 +3293,7 @@
         <v>177</v>
       </c>
       <c r="B45">
-        <v>0.5199698568198945</v>
+        <v>0.5850340136054422</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3301,7 +3301,7 @@
         <v>178</v>
       </c>
       <c r="B46">
-        <v>0.4494584837545126</v>
+        <v>0.5377969762419006</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3309,7 +3309,7 @@
         <v>179</v>
       </c>
       <c r="B47">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3317,7 +3317,7 @@
         <v>180</v>
       </c>
       <c r="B48">
-        <v>0.4709141274238227</v>
+        <v>0.5357710651828299</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3325,7 +3325,7 @@
         <v>181</v>
       </c>
       <c r="B49">
-        <v>0.4646840148698885</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3333,7 +3333,7 @@
         <v>182</v>
       </c>
       <c r="B50">
-        <v>0.4836512261580381</v>
+        <v>0.5583596214511041</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3341,7 +3341,7 @@
         <v>183</v>
       </c>
       <c r="B51">
-        <v>0.5208333333333334</v>
+        <v>0.6097560975609756</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3349,7 +3349,7 @@
         <v>184</v>
       </c>
       <c r="B52">
-        <v>0.5071428571428571</v>
+        <v>0.5949367088607594</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3357,7 +3357,7 @@
         <v>185</v>
       </c>
       <c r="B53">
-        <v>0.5538461538461539</v>
+        <v>0.6467065868263473</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3365,7 +3365,7 @@
         <v>186</v>
       </c>
       <c r="B54">
-        <v>0.4347826086956522</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3373,7 +3373,7 @@
         <v>187</v>
       </c>
       <c r="B55">
-        <v>0.5010570824524313</v>
+        <v>0.5690072639225182</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3381,7 +3381,7 @@
         <v>188</v>
       </c>
       <c r="B56">
-        <v>0.4752321981424149</v>
+        <v>0.5575868372943327</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3389,7 +3389,7 @@
         <v>189</v>
       </c>
       <c r="B57">
-        <v>0.4630914826498423</v>
+        <v>0.5045806906272022</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3397,7 +3397,7 @@
         <v>190</v>
       </c>
       <c r="B58">
-        <v>0.4875491480996068</v>
+        <v>0.5672782874617737</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3405,7 +3405,7 @@
         <v>191</v>
       </c>
       <c r="B59">
-        <v>0.4317817014446228</v>
+        <v>0.5358565737051793</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3413,7 +3413,7 @@
         <v>192</v>
       </c>
       <c r="B60">
-        <v>0.4777070063694268</v>
+        <v>0.5576208178438662</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3421,7 +3421,7 @@
         <v>193</v>
       </c>
       <c r="B61">
-        <v>0.4629854368932039</v>
+        <v>0.5301966292134831</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3429,7 +3429,7 @@
         <v>194</v>
       </c>
       <c r="B62">
-        <v>0.4770468528159015</v>
+        <v>0.569971671388102</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3437,7 +3437,7 @@
         <v>195</v>
       </c>
       <c r="B63">
-        <v>0.4530831099195711</v>
+        <v>0.5248447204968945</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3445,7 +3445,7 @@
         <v>196</v>
       </c>
       <c r="B64">
-        <v>0.5017195261750096</v>
+        <v>0.5653123634775011</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -3453,7 +3453,7 @@
         <v>197</v>
       </c>
       <c r="B65">
-        <v>0.4611111111111111</v>
+        <v>0.532051282051282</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -3461,7 +3461,7 @@
         <v>198</v>
       </c>
       <c r="B66">
-        <v>0.5222405271828665</v>
+        <v>0.6042065009560229</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3469,7 +3469,7 @@
         <v>199</v>
       </c>
       <c r="B67">
-        <v>0.4626865671641791</v>
+        <v>0.543859649122807</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3477,7 +3477,7 @@
         <v>200</v>
       </c>
       <c r="B68">
-        <v>0.4639328063241107</v>
+        <v>0.5327635327635327</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3485,7 +3485,7 @@
         <v>201</v>
       </c>
       <c r="B69">
-        <v>0.4154471544715447</v>
+        <v>0.4870813397129187</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -3493,7 +3493,7 @@
         <v>202</v>
       </c>
       <c r="B70">
-        <v>0.4868804664723032</v>
+        <v>0.6887966804979253</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -3501,7 +3501,7 @@
         <v>203</v>
       </c>
       <c r="B71">
-        <v>0.4478063540090771</v>
+        <v>0.5623800383877159</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -3509,7 +3509,7 @@
         <v>204</v>
       </c>
       <c r="B72">
-        <v>0.4545954870665933</v>
+        <v>0.5579163810829335</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -3517,7 +3517,7 @@
         <v>205</v>
       </c>
       <c r="B73">
-        <v>0.4895104895104895</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3525,7 +3525,7 @@
         <v>206</v>
       </c>
       <c r="B74">
-        <v>0.4700443786982249</v>
+        <v>0.5276831345826235</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -3533,7 +3533,7 @@
         <v>207</v>
       </c>
       <c r="B75">
-        <v>0.4875</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3541,7 +3541,7 @@
         <v>208</v>
       </c>
       <c r="B76">
-        <v>0.5</v>
+        <v>0.5733333333333334</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3549,7 +3549,7 @@
         <v>209</v>
       </c>
       <c r="B77">
-        <v>0.4928762243989314</v>
+        <v>0.5621483375959079</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3557,7 +3557,7 @@
         <v>210</v>
       </c>
       <c r="B78">
-        <v>0.4622535211267605</v>
+        <v>0.5572019297036527</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3565,7 +3565,7 @@
         <v>211</v>
       </c>
       <c r="B79">
-        <v>0.4810126582278481</v>
+        <v>0.5635593220338984</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3573,7 +3573,7 @@
         <v>212</v>
       </c>
       <c r="B80">
-        <v>0.4580838323353293</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3581,7 +3581,7 @@
         <v>213</v>
       </c>
       <c r="B81">
-        <v>0.5287187039764359</v>
+        <v>0.6033613445378151</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3589,7 +3589,7 @@
         <v>214</v>
       </c>
       <c r="B82">
-        <v>0.5</v>
+        <v>0.5814432989690722</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3597,7 +3597,7 @@
         <v>215</v>
       </c>
       <c r="B83">
-        <v>0.4731182795698925</v>
+        <v>0.5641025641025641</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -3605,7 +3605,7 @@
         <v>216</v>
       </c>
       <c r="B84">
-        <v>0.4716981132075472</v>
+        <v>0.5853658536585366</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3613,7 +3613,7 @@
         <v>217</v>
       </c>
       <c r="B85">
-        <v>0.4785478547854786</v>
+        <v>0.5797101449275363</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -3621,7 +3621,7 @@
         <v>218</v>
       </c>
       <c r="B86">
-        <v>0.4549237170596394</v>
+        <v>0.551433389544688</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3629,7 +3629,7 @@
         <v>219</v>
       </c>
       <c r="B87">
-        <v>0.4554865424430642</v>
+        <v>0.5513784461152882</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -3637,7 +3637,7 @@
         <v>220</v>
       </c>
       <c r="B88">
-        <v>0.4780876494023905</v>
+        <v>0.5571095571095571</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3645,7 +3645,7 @@
         <v>221</v>
       </c>
       <c r="B89">
-        <v>0.4818840579710145</v>
+        <v>0.5518672199170125</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3653,7 +3653,7 @@
         <v>222</v>
       </c>
       <c r="B90">
-        <v>0.4349157733537519</v>
+        <v>0.5348399246704332</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -3661,7 +3661,7 @@
         <v>223</v>
       </c>
       <c r="B91">
-        <v>0.4927536231884058</v>
+        <v>0.5862068965517241</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3669,7 +3669,7 @@
         <v>224</v>
       </c>
       <c r="B92">
-        <v>0.5005107252298263</v>
+        <v>0.5643105446118193</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -3677,7 +3677,7 @@
         <v>225</v>
       </c>
       <c r="B93">
-        <v>0.4767123287671233</v>
+        <v>0.5523809523809524</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -3685,7 +3685,7 @@
         <v>226</v>
       </c>
       <c r="B94">
-        <v>0.4572425828970332</v>
+        <v>0.55863539445629</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -3693,7 +3693,7 @@
         <v>227</v>
       </c>
       <c r="B95">
-        <v>0.5360576923076923</v>
+        <v>0.6261127596439169</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -3701,7 +3701,7 @@
         <v>228</v>
       </c>
       <c r="B96">
-        <v>0.4730538922155689</v>
+        <v>0.5589080459770115</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3709,7 +3709,7 @@
         <v>229</v>
       </c>
       <c r="B97">
-        <v>0.4651162790697674</v>
+        <v>0.5797101449275363</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -3717,7 +3717,7 @@
         <v>230</v>
       </c>
       <c r="B98">
-        <v>0.51875</v>
+        <v>0.578397212543554</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -3725,7 +3725,7 @@
         <v>231</v>
       </c>
       <c r="B99">
-        <v>0.4887640449438202</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -3733,7 +3733,7 @@
         <v>232</v>
       </c>
       <c r="B100">
-        <v>0.4338624338624338</v>
+        <v>0.5082644628099173</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -3741,7 +3741,7 @@
         <v>233</v>
       </c>
       <c r="B101">
-        <v>0.5167682926829268</v>
+        <v>0.5989399293286219</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -3749,7 +3749,7 @@
         <v>234</v>
       </c>
       <c r="B102">
-        <v>0.4928</v>
+        <v>0.599609375</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -3757,7 +3757,7 @@
         <v>235</v>
       </c>
       <c r="B103">
-        <v>0.4826302729528536</v>
+        <v>0.5380359612724758</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -3765,7 +3765,7 @@
         <v>236</v>
       </c>
       <c r="B104">
-        <v>0.49800796812749</v>
+        <v>0.5827505827505828</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -3773,7 +3773,7 @@
         <v>237</v>
       </c>
       <c r="B105">
-        <v>0.521978021978022</v>
+        <v>0.5855670103092784</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -3781,7 +3781,7 @@
         <v>238</v>
       </c>
       <c r="B106">
-        <v>0.4379562043795621</v>
+        <v>0.4878048780487805</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -3789,7 +3789,7 @@
         <v>239</v>
       </c>
       <c r="B107">
-        <v>0.4782608695652174</v>
+        <v>0.5392156862745098</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -3797,7 +3797,7 @@
         <v>240</v>
       </c>
       <c r="B108">
-        <v>0.407981220657277</v>
+        <v>0.4708446866485014</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -3805,7 +3805,7 @@
         <v>241</v>
       </c>
       <c r="B109">
-        <v>0.4827586206896552</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -3813,7 +3813,7 @@
         <v>242</v>
       </c>
       <c r="B110">
-        <v>0.4678899082568808</v>
+        <v>0.5334207077326344</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -3821,7 +3821,7 @@
         <v>243</v>
       </c>
       <c r="B111">
-        <v>0.4780334728033473</v>
+        <v>0.5554202192448234</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -3829,7 +3829,7 @@
         <v>244</v>
       </c>
       <c r="B112">
-        <v>0.4736842105263158</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -3837,7 +3837,7 @@
         <v>245</v>
       </c>
       <c r="B113">
-        <v>0.4386252045826514</v>
+        <v>0.5297619047619048</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3845,7 +3845,7 @@
         <v>246</v>
       </c>
       <c r="B114">
-        <v>0.5116279069767442</v>
+        <v>0.5936794582392777</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -3853,7 +3853,7 @@
         <v>247</v>
       </c>
       <c r="B115">
-        <v>0.4887063655030801</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -3861,7 +3861,7 @@
         <v>248</v>
       </c>
       <c r="B116">
-        <v>0.5250596658711217</v>
+        <v>0.6066481994459834</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3869,7 +3869,7 @@
         <v>249</v>
       </c>
       <c r="B117">
-        <v>0.5177809388335705</v>
+        <v>0.6076794657762938</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3877,7 +3877,7 @@
         <v>250</v>
       </c>
       <c r="B118">
-        <v>0.5030927835051546</v>
+        <v>0.5907990314769975</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -3885,7 +3885,7 @@
         <v>251</v>
       </c>
       <c r="B119">
-        <v>0.4776119402985075</v>
+        <v>0.5606326889279437</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -3893,7 +3893,7 @@
         <v>252</v>
       </c>
       <c r="B120">
-        <v>0.476280834914611</v>
+        <v>0.5518763796909493</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3901,7 +3901,7 @@
         <v>253</v>
       </c>
       <c r="B121">
-        <v>0.4713375796178344</v>
+        <v>0.5580693815987934</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -3909,7 +3909,7 @@
         <v>254</v>
       </c>
       <c r="B122">
-        <v>0.456359102244389</v>
+        <v>0.629757785467128</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -3917,7 +3917,7 @@
         <v>255</v>
       </c>
       <c r="B123">
-        <v>0.530920060331825</v>
+        <v>0.6065857885615251</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -3925,7 +3925,7 @@
         <v>256</v>
       </c>
       <c r="B124">
-        <v>0.4797687861271676</v>
+        <v>0.5570469798657718</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -3933,7 +3933,7 @@
         <v>257</v>
       </c>
       <c r="B125">
-        <v>0.4936170212765957</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -3941,7 +3941,7 @@
         <v>258</v>
       </c>
       <c r="B126">
-        <v>0.4741935483870968</v>
+        <v>0.55893536121673</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -3949,7 +3949,7 @@
         <v>259</v>
       </c>
       <c r="B127">
-        <v>0.490280777537797</v>
+        <v>0.583547557840617</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -3957,7 +3957,7 @@
         <v>260</v>
       </c>
       <c r="B128">
-        <v>0.4701834862385321</v>
+        <v>0.5501355013550135</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -3965,7 +3965,7 @@
         <v>261</v>
       </c>
       <c r="B129">
-        <v>0.465359477124183</v>
+        <v>0.5603174603174603</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3973,7 +3973,7 @@
         <v>262</v>
       </c>
       <c r="B130">
-        <v>0.5402298850574713</v>
+        <v>0.5875</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -3981,7 +3981,7 @@
         <v>263</v>
       </c>
       <c r="B131">
-        <v>0.4575725026852847</v>
+        <v>0.5332496863237139</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3989,7 +3989,7 @@
         <v>264</v>
       </c>
       <c r="B132">
-        <v>0.4875621890547264</v>
+        <v>0.5672514619883041</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -3997,7 +3997,7 @@
         <v>265</v>
       </c>
       <c r="B133">
-        <v>0.5019455252918288</v>
+        <v>0.5854214123006833</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -4005,7 +4005,7 @@
         <v>266</v>
       </c>
       <c r="B134">
-        <v>0.4517437145174372</v>
+        <v>0.5254716981132076</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -4013,7 +4013,7 @@
         <v>267</v>
       </c>
       <c r="B135">
-        <v>0.38</v>
+        <v>0.4634146341463415</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -4021,7 +4021,7 @@
         <v>268</v>
       </c>
       <c r="B136">
-        <v>0.4444444444444444</v>
+        <v>0.4968944099378882</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -4029,7 +4029,7 @@
         <v>269</v>
       </c>
       <c r="B137">
-        <v>0.4723404255319149</v>
+        <v>0.5763016157989228</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -4037,7 +4037,7 @@
         <v>270</v>
       </c>
       <c r="B138">
-        <v>0.4597315436241611</v>
+        <v>0.5524193548387096</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -4045,7 +4045,7 @@
         <v>271</v>
       </c>
       <c r="B139">
-        <v>0.4836601307189543</v>
+        <v>0.5401459854014599</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -4053,7 +4053,7 @@
         <v>272</v>
       </c>
       <c r="B140">
-        <v>0.485024154589372</v>
+        <v>0.5823665893271461</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -4061,7 +4061,7 @@
         <v>273</v>
       </c>
       <c r="B141">
-        <v>0.4724220623501199</v>
+        <v>0.5584045584045584</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -4069,7 +4069,7 @@
         <v>274</v>
       </c>
       <c r="B142">
-        <v>0.5061349693251533</v>
+        <v>0.5857142857142857</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -4077,7 +4077,7 @@
         <v>275</v>
       </c>
       <c r="B143">
-        <v>0.5</v>
+        <v>0.5812101910828026</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -4085,7 +4085,7 @@
         <v>276</v>
       </c>
       <c r="B144">
-        <v>0.5048661800486618</v>
+        <v>0.5763888888888888</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -4093,7 +4093,7 @@
         <v>277</v>
       </c>
       <c r="B145">
-        <v>0.4670184696569921</v>
+        <v>0.5412844036697247</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -4101,7 +4101,7 @@
         <v>278</v>
       </c>
       <c r="B146">
-        <v>0.5064308681672026</v>
+        <v>0.6081081081081081</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -4109,7 +4109,7 @@
         <v>279</v>
       </c>
       <c r="B147">
-        <v>0.4046140195208518</v>
+        <v>0.4774396642182581</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -4117,7 +4117,7 @@
         <v>280</v>
       </c>
       <c r="B148">
-        <v>0.4449244060475162</v>
+        <v>0.5073891625615764</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -4125,7 +4125,7 @@
         <v>281</v>
       </c>
       <c r="B149">
-        <v>0.4487179487179487</v>
+        <v>0.5147058823529411</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -4133,7 +4133,7 @@
         <v>282</v>
       </c>
       <c r="B150">
-        <v>0.4915316642120766</v>
+        <v>0.5686444348202685</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -4141,7 +4141,7 @@
         <v>283</v>
       </c>
       <c r="B151">
-        <v>0.459954233409611</v>
+        <v>0.5388739946380697</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -4149,7 +4149,7 @@
         <v>284</v>
       </c>
       <c r="B152">
-        <v>0.3953488372093023</v>
+        <v>0.4473684210526316</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -4157,7 +4157,7 @@
         <v>285</v>
       </c>
       <c r="B153">
-        <v>0.5030864197530864</v>
+        <v>0.5719298245614035</v>
       </c>
     </row>
   </sheetData>
@@ -4186,7 +4186,7 @@
         <v>286</v>
       </c>
       <c r="B2">
-        <v>0.4208144796380091</v>
+        <v>0.5027027027027027</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4194,7 +4194,7 @@
         <v>287</v>
       </c>
       <c r="B3">
-        <v>0.5234159779614325</v>
+        <v>0.5851393188854489</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4202,7 +4202,7 @@
         <v>288</v>
       </c>
       <c r="B4">
-        <v>0.498812351543943</v>
+        <v>0.5514511873350924</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4210,7 +4210,7 @@
         <v>289</v>
       </c>
       <c r="B5">
-        <v>0.5531914893617021</v>
+        <v>0.6190476190476191</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4218,7 +4218,7 @@
         <v>290</v>
       </c>
       <c r="B6">
-        <v>0.4815618221258134</v>
+        <v>0.654357459379616</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4226,7 +4226,7 @@
         <v>291</v>
       </c>
       <c r="B7">
-        <v>0.5024449877750611</v>
+        <v>0.582723279648609</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4234,7 +4234,7 @@
         <v>292</v>
       </c>
       <c r="B8">
-        <v>0.4685138539042821</v>
+        <v>0.5525114155251142</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4242,7 +4242,7 @@
         <v>293</v>
       </c>
       <c r="B9">
-        <v>0.4287581699346405</v>
+        <v>0.5046296296296297</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4250,7 +4250,7 @@
         <v>294</v>
       </c>
       <c r="B10">
-        <v>0.4867924528301887</v>
+        <v>0.5608695652173913</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4258,7 +4258,7 @@
         <v>295</v>
       </c>
       <c r="B11">
-        <v>0.4314214463840399</v>
+        <v>0.5068493150684932</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4266,7 +4266,7 @@
         <v>296</v>
       </c>
       <c r="B12">
-        <v>0.570222563315426</v>
+        <v>0.6382795698924731</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4274,7 +4274,7 @@
         <v>297</v>
       </c>
       <c r="B13">
-        <v>0.468562874251497</v>
+        <v>0.5316239316239316</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4282,7 +4282,7 @@
         <v>298</v>
       </c>
       <c r="B14">
-        <v>0.5035561877667141</v>
+        <v>0.5912897822445561</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4290,7 +4290,7 @@
         <v>299</v>
       </c>
       <c r="B15">
-        <v>0.4692118226600985</v>
+        <v>0.5627769571639586</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4298,7 +4298,7 @@
         <v>300</v>
       </c>
       <c r="B16">
-        <v>0.4310344827586207</v>
+        <v>0.4926108374384237</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4306,7 +4306,7 @@
         <v>301</v>
       </c>
       <c r="B17">
-        <v>0.4984646878198567</v>
+        <v>0.5613608748481167</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4314,7 +4314,7 @@
         <v>302</v>
       </c>
       <c r="B18">
-        <v>0.4655482324745356</v>
+        <v>0.5609579100145138</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4322,7 +4322,7 @@
         <v>303</v>
       </c>
       <c r="B19">
-        <v>0.4297520661157025</v>
+        <v>0.5012048192771085</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4330,7 +4330,7 @@
         <v>304</v>
       </c>
       <c r="B20">
-        <v>0.4743589743589743</v>
+        <v>0.5589123867069486</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4338,7 +4338,7 @@
         <v>305</v>
       </c>
       <c r="B21">
-        <v>0.4834123222748815</v>
+        <v>0.5873320537428023</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4346,7 +4346,7 @@
         <v>306</v>
       </c>
       <c r="B22">
-        <v>0.4347357065803668</v>
+        <v>0.5031210986267166</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4354,7 +4354,7 @@
         <v>307</v>
       </c>
       <c r="B23">
-        <v>0.4650735294117647</v>
+        <v>0.5281837160751566</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4362,7 +4362,7 @@
         <v>308</v>
       </c>
       <c r="B24">
-        <v>0.4537566554920134</v>
+        <v>0.5280924855491329</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4370,7 +4370,7 @@
         <v>309</v>
       </c>
       <c r="B25">
-        <v>0.4902597402597403</v>
+        <v>0.5806295399515738</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4378,7 +4378,7 @@
         <v>310</v>
       </c>
       <c r="B26">
-        <v>0.4404145077720207</v>
+        <v>0.6021505376344086</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4386,7 +4386,7 @@
         <v>311</v>
       </c>
       <c r="B27">
-        <v>0.4329710144927536</v>
+        <v>0.5252747252747253</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4394,7 +4394,7 @@
         <v>312</v>
       </c>
       <c r="B28">
-        <v>0.4808219178082192</v>
+        <v>0.5792988313856428</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4402,7 +4402,7 @@
         <v>313</v>
       </c>
       <c r="B29">
-        <v>0.5464968152866242</v>
+        <v>0.6578947368421053</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4410,7 +4410,7 @@
         <v>314</v>
       </c>
       <c r="B30">
-        <v>0.4188267394270123</v>
+        <v>0.5261324041811847</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4418,7 +4418,7 @@
         <v>315</v>
       </c>
       <c r="B31">
-        <v>0.5026178010471204</v>
+        <v>0.5748502994011976</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4426,7 +4426,7 @@
         <v>316</v>
       </c>
       <c r="B32">
-        <v>0.4706684856753069</v>
+        <v>0.555735056542811</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4434,7 +4434,7 @@
         <v>317</v>
       </c>
       <c r="B33">
-        <v>0.4959349593495935</v>
+        <v>0.5754716981132075</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4442,7 +4442,7 @@
         <v>318</v>
       </c>
       <c r="B34">
-        <v>0.473170731707317</v>
+        <v>0.5606936416184971</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4450,7 +4450,7 @@
         <v>319</v>
       </c>
       <c r="B35">
-        <v>0.5181347150259067</v>
+        <v>0.591715976331361</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4458,7 +4458,7 @@
         <v>320</v>
       </c>
       <c r="B36">
-        <v>0.4578606158833063</v>
+        <v>0.5430784123910939</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4466,7 +4466,7 @@
         <v>321</v>
       </c>
       <c r="B37">
-        <v>0.4572564612326044</v>
+        <v>0.5386416861826698</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4474,7 +4474,7 @@
         <v>322</v>
       </c>
       <c r="B38">
-        <v>0.4610564010743062</v>
+        <v>0.5567567567567567</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4482,7 +4482,7 @@
         <v>323</v>
       </c>
       <c r="B39">
-        <v>0.4800995024875622</v>
+        <v>0.5676470588235294</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4490,7 +4490,7 @@
         <v>324</v>
       </c>
       <c r="B40">
-        <v>0.4125</v>
+        <v>0.5038167938931297</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4498,7 +4498,7 @@
         <v>325</v>
       </c>
       <c r="B41">
-        <v>0.4938775510204081</v>
+        <v>0.5535224153705398</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4506,7 +4506,7 @@
         <v>326</v>
       </c>
       <c r="B42">
-        <v>0.4834905660377358</v>
+        <v>0.5551020408163265</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4514,7 +4514,7 @@
         <v>327</v>
       </c>
       <c r="B43">
-        <v>0.4509803921568628</v>
+        <v>0.5139664804469274</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4522,7 +4522,7 @@
         <v>328</v>
       </c>
       <c r="B44">
-        <v>0.4411764705882353</v>
+        <v>0.531496062992126</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4530,7 +4530,7 @@
         <v>329</v>
       </c>
       <c r="B45">
-        <v>0.4932432432432433</v>
+        <v>0.5778364116094987</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4538,7 +4538,7 @@
         <v>330</v>
       </c>
       <c r="B46">
-        <v>0.4288389513108614</v>
+        <v>0.5018001800180018</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4546,7 +4546,7 @@
         <v>331</v>
       </c>
       <c r="B47">
-        <v>0.46875</v>
+        <v>0.5487804878048781</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4554,7 +4554,7 @@
         <v>332</v>
       </c>
       <c r="B48">
-        <v>0.4301075268817204</v>
+        <v>0.4927835051546392</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4562,7 +4562,7 @@
         <v>333</v>
       </c>
       <c r="B49">
-        <v>0.53125</v>
+        <v>0.5895953757225434</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4570,7 +4570,7 @@
         <v>334</v>
       </c>
       <c r="B50">
-        <v>0.4229390681003584</v>
+        <v>0.5086206896551724</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4578,7 +4578,7 @@
         <v>335</v>
       </c>
       <c r="B51">
-        <v>0.4820819112627986</v>
+        <v>0.5621242484969939</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4586,7 +4586,7 @@
         <v>336</v>
       </c>
       <c r="B52">
-        <v>0.4765957446808511</v>
+        <v>0.5628140703517588</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4594,7 +4594,7 @@
         <v>337</v>
       </c>
       <c r="B53">
-        <v>0.4900990099009901</v>
+        <v>0.5722543352601156</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4602,7 +4602,7 @@
         <v>338</v>
       </c>
       <c r="B54">
-        <v>0.4581320450885668</v>
+        <v>0.5508228460793805</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4610,7 +4610,7 @@
         <v>339</v>
       </c>
       <c r="B55">
-        <v>0.5272727272727272</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4618,7 +4618,7 @@
         <v>340</v>
       </c>
       <c r="B56">
-        <v>0.5030581039755352</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4626,7 +4626,7 @@
         <v>341</v>
       </c>
       <c r="B57">
-        <v>0.4206815511163337</v>
+        <v>0.4992987377279102</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4634,7 +4634,7 @@
         <v>342</v>
       </c>
       <c r="B58">
-        <v>0.4783236994219653</v>
+        <v>0.5316045380875203</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4642,7 +4642,7 @@
         <v>343</v>
       </c>
       <c r="B59">
-        <v>0.4926470588235294</v>
+        <v>0.5826086956521739</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4650,7 +4650,7 @@
         <v>344</v>
       </c>
       <c r="B60">
-        <v>0.4810126582278481</v>
+        <v>0.5748987854251012</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4658,7 +4658,7 @@
         <v>345</v>
       </c>
       <c r="B61">
-        <v>0.5</v>
+        <v>0.594488188976378</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4666,7 +4666,7 @@
         <v>346</v>
       </c>
       <c r="B62">
-        <v>0.4848066298342542</v>
+        <v>0.5690515806988353</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4674,7 +4674,7 @@
         <v>347</v>
       </c>
       <c r="B63">
-        <v>0.4137931034482759</v>
+        <v>0.5136186770428015</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4682,7 +4682,7 @@
         <v>348</v>
       </c>
       <c r="B64">
-        <v>0.5066828675577156</v>
+        <v>0.5948644793152639</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4690,7 +4690,7 @@
         <v>349</v>
       </c>
       <c r="B65">
-        <v>0.510803324099723</v>
+        <v>0.5741792929292929</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4698,7 +4698,7 @@
         <v>350</v>
       </c>
       <c r="B66">
-        <v>0.4435483870967742</v>
+        <v>0.5225653206650831</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4706,7 +4706,7 @@
         <v>351</v>
       </c>
       <c r="B67">
-        <v>0.4802744425385935</v>
+        <v>0.561122244488978</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4714,7 +4714,7 @@
         <v>352</v>
       </c>
       <c r="B68">
-        <v>0.4976744186046512</v>
+        <v>0.5881057268722467</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4722,7 +4722,7 @@
         <v>353</v>
       </c>
       <c r="B69">
-        <v>0.4798518841211065</v>
+        <v>0.5489350912778904</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4730,7 +4730,7 @@
         <v>354</v>
       </c>
       <c r="B70">
-        <v>0.5769230769230769</v>
+        <v>0.6521739130434783</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4738,7 +4738,7 @@
         <v>355</v>
       </c>
       <c r="B71">
-        <v>0.4789644012944984</v>
+        <v>0.5569948186528497</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4746,7 +4746,7 @@
         <v>356</v>
       </c>
       <c r="B72">
-        <v>0.4517453798767967</v>
+        <v>0.5289156626506024</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4754,7 +4754,7 @@
         <v>357</v>
       </c>
       <c r="B73">
-        <v>0.4666666666666667</v>
+        <v>0.5434210526315789</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4762,7 +4762,7 @@
         <v>358</v>
       </c>
       <c r="B74">
-        <v>0.5083333333333333</v>
+        <v>0.601593625498008</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4770,7 +4770,7 @@
         <v>359</v>
       </c>
       <c r="B75">
-        <v>0.5183374083129584</v>
+        <v>0.6028571428571429</v>
       </c>
     </row>
   </sheetData>
@@ -4799,7 +4799,7 @@
         <v>360</v>
       </c>
       <c r="B2">
-        <v>0.4490909090909091</v>
+        <v>0.5089408528198074</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4807,7 +4807,7 @@
         <v>361</v>
       </c>
       <c r="B3">
-        <v>0.4706840390879479</v>
+        <v>0.5411985018726592</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4815,7 +4815,7 @@
         <v>362</v>
       </c>
       <c r="B4">
-        <v>0.4973890339425587</v>
+        <v>0.5953125</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4823,7 +4823,7 @@
         <v>363</v>
       </c>
       <c r="B5">
-        <v>0.4977777777777778</v>
+        <v>0.5894736842105263</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4831,7 +4831,7 @@
         <v>364</v>
       </c>
       <c r="B6">
-        <v>0.4126625211984172</v>
+        <v>0.4738237243207422</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4839,7 +4839,7 @@
         <v>365</v>
       </c>
       <c r="B7">
-        <v>0.5059347181008902</v>
+        <v>0.5798611111111112</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4847,7 +4847,7 @@
         <v>366</v>
       </c>
       <c r="B8">
-        <v>0.5265486725663717</v>
+        <v>0.6062176165803109</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4855,7 +4855,7 @@
         <v>367</v>
       </c>
       <c r="B9">
-        <v>0.5148936170212766</v>
+        <v>0.6132315521628499</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4863,7 +4863,7 @@
         <v>368</v>
       </c>
       <c r="B10">
-        <v>0.4903846153846154</v>
+        <v>0.5702247191011236</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4871,7 +4871,7 @@
         <v>369</v>
       </c>
       <c r="B11">
-        <v>0.4646118721461187</v>
+        <v>0.564673157162726</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4879,7 +4879,7 @@
         <v>370</v>
       </c>
       <c r="B12">
-        <v>0.4598393574297189</v>
+        <v>0.5330188679245284</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4887,7 +4887,7 @@
         <v>371</v>
       </c>
       <c r="B13">
-        <v>0.5025062656641605</v>
+        <v>0.6030075187969924</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4895,7 +4895,7 @@
         <v>372</v>
       </c>
       <c r="B14">
-        <v>0.4550359712230216</v>
+        <v>0.5249480249480249</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4903,7 +4903,7 @@
         <v>373</v>
       </c>
       <c r="B15">
-        <v>0.4483775811209439</v>
+        <v>0.5283687943262412</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4911,7 +4911,7 @@
         <v>374</v>
       </c>
       <c r="B16">
-        <v>0.471386040357261</v>
+        <v>0.5635643564356435</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4919,7 +4919,7 @@
         <v>375</v>
       </c>
       <c r="B17">
-        <v>0.4778761061946903</v>
+        <v>0.5659670164917541</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4927,7 +4927,7 @@
         <v>376</v>
       </c>
       <c r="B18">
-        <v>0.436046511627907</v>
+        <v>0.4918032786885246</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4935,7 +4935,7 @@
         <v>377</v>
       </c>
       <c r="B19">
-        <v>0.5039817974971559</v>
+        <v>0.5823451910408433</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4943,7 +4943,7 @@
         <v>378</v>
       </c>
       <c r="B20">
-        <v>0.4017094017094017</v>
+        <v>0.483704974271012</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4951,7 +4951,7 @@
         <v>379</v>
       </c>
       <c r="B21">
-        <v>0.4689100219458668</v>
+        <v>0.5441426146010186</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4959,7 +4959,7 @@
         <v>380</v>
       </c>
       <c r="B22">
-        <v>0.4528735632183908</v>
+        <v>0.5474860335195531</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4967,7 +4967,7 @@
         <v>381</v>
       </c>
       <c r="B23">
-        <v>0.4934426229508197</v>
+        <v>0.5874263261296661</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4975,7 +4975,7 @@
         <v>382</v>
       </c>
       <c r="B24">
-        <v>0.5091463414634146</v>
+        <v>0.6234413965087282</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4983,7 +4983,7 @@
         <v>383</v>
       </c>
       <c r="B25">
-        <v>0.4259259259259259</v>
+        <v>0.5080321285140562</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4991,7 +4991,7 @@
         <v>384</v>
       </c>
       <c r="B26">
-        <v>0.4760147601476015</v>
+        <v>0.5939675174013921</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4999,7 +4999,7 @@
         <v>385</v>
       </c>
       <c r="B27">
-        <v>0.4921465968586388</v>
+        <v>0.5927099841521395</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5007,7 +5007,7 @@
         <v>386</v>
       </c>
       <c r="B28">
-        <v>0.5258278145695364</v>
+        <v>0.6301587301587301</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5015,7 +5015,7 @@
         <v>387</v>
       </c>
       <c r="B29">
-        <v>0.4938080495356037</v>
+        <v>0.5628318584070796</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -5023,7 +5023,7 @@
         <v>388</v>
       </c>
       <c r="B30">
-        <v>0.4355362946912243</v>
+        <v>0.5056603773584906</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -5031,7 +5031,7 @@
         <v>389</v>
       </c>
       <c r="B31">
-        <v>0.4555052790346908</v>
+        <v>0.5364120781527532</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5039,7 +5039,7 @@
         <v>390</v>
       </c>
       <c r="B32">
-        <v>0.4855818743563337</v>
+        <v>0.5610778443113772</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -5047,7 +5047,7 @@
         <v>391</v>
       </c>
       <c r="B33">
-        <v>0.4669117647058824</v>
+        <v>0.5772727272727273</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5055,7 +5055,7 @@
         <v>392</v>
       </c>
       <c r="B34">
-        <v>0.5097024579560155</v>
+        <v>0.6109375</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -5063,7 +5063,7 @@
         <v>393</v>
       </c>
       <c r="B35">
-        <v>0.4275862068965517</v>
+        <v>0.5330459770114943</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5071,7 +5071,7 @@
         <v>394</v>
       </c>
       <c r="B36">
-        <v>0.4314606741573034</v>
+        <v>0.514745308310992</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5079,7 +5079,7 @@
         <v>395</v>
       </c>
       <c r="B37">
-        <v>0.6028119507908611</v>
+        <v>0.692929292929293</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5087,7 +5087,7 @@
         <v>396</v>
       </c>
       <c r="B38">
-        <v>0.4612403100775194</v>
+        <v>0.5947302383939774</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5095,7 +5095,7 @@
         <v>397</v>
       </c>
       <c r="B39">
-        <v>0.4929282346778418</v>
+        <v>0.5725658297611758</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -5103,7 +5103,7 @@
         <v>398</v>
       </c>
       <c r="B40">
-        <v>0.4882154882154882</v>
+        <v>0.5451127819548872</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -5111,7 +5111,7 @@
         <v>399</v>
       </c>
       <c r="B41">
-        <v>0.5144827586206897</v>
+        <v>0.5920634920634921</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -5119,7 +5119,7 @@
         <v>400</v>
       </c>
       <c r="B42">
-        <v>0.5818181818181818</v>
+        <v>0.6530612244897959</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -5127,7 +5127,7 @@
         <v>401</v>
       </c>
       <c r="B43">
-        <v>0.4479638009049774</v>
+        <v>0.5302073940486925</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -5135,7 +5135,7 @@
         <v>402</v>
       </c>
       <c r="B44">
-        <v>0.4526748971193416</v>
+        <v>0.5378973105134475</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -5143,7 +5143,7 @@
         <v>403</v>
       </c>
       <c r="B45">
-        <v>0.5138461538461538</v>
+        <v>0.6151012891344383</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -5151,7 +5151,7 @@
         <v>404</v>
       </c>
       <c r="B46">
-        <v>0.4873817034700316</v>
+        <v>0.5645013723696248</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -5159,7 +5159,7 @@
         <v>405</v>
       </c>
       <c r="B47">
-        <v>0.4587912087912088</v>
+        <v>0.5496688741721855</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -5167,7 +5167,7 @@
         <v>406</v>
       </c>
       <c r="B48">
-        <v>0.3962264150943396</v>
+        <v>0.4745762711864407</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5175,7 +5175,7 @@
         <v>407</v>
       </c>
       <c r="B49">
-        <v>0.4736842105263158</v>
+        <v>0.5563186813186813</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -5183,7 +5183,7 @@
         <v>408</v>
       </c>
       <c r="B50">
-        <v>0.5111464968152867</v>
+        <v>0.5922509225092251</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -5191,7 +5191,7 @@
         <v>409</v>
       </c>
       <c r="B51">
-        <v>0.4363438520130577</v>
+        <v>0.5284015852047557</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -5199,7 +5199,7 @@
         <v>410</v>
       </c>
       <c r="B52">
-        <v>0.5092975206611571</v>
+        <v>0.6027060270602707</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -5207,7 +5207,7 @@
         <v>411</v>
       </c>
       <c r="B53">
-        <v>0.5084175084175084</v>
+        <v>0.5908496732026144</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -5215,7 +5215,7 @@
         <v>412</v>
       </c>
       <c r="B54">
-        <v>0.4992481203007519</v>
+        <v>0.5974729241877257</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -5223,7 +5223,7 @@
         <v>413</v>
       </c>
       <c r="B55">
-        <v>0.5078088026502603</v>
+        <v>0.5786608600979859</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5231,7 +5231,7 @@
         <v>414</v>
       </c>
       <c r="B56">
-        <v>0.4337349397590362</v>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -5239,7 +5239,7 @@
         <v>415</v>
       </c>
       <c r="B57">
-        <v>0.4751830756712775</v>
+        <v>0.5474178403755868</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5247,7 +5247,7 @@
         <v>416</v>
       </c>
       <c r="B58">
-        <v>0.5064308681672026</v>
+        <v>0.6178217821782178</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -5255,7 +5255,7 @@
         <v>417</v>
       </c>
       <c r="B59">
-        <v>0.5030864197530864</v>
+        <v>0.5926605504587156</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -5263,7 +5263,7 @@
         <v>418</v>
       </c>
       <c r="B60">
-        <v>0.4963562753036437</v>
+        <v>0.5694315004659832</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -5271,7 +5271,7 @@
         <v>419</v>
       </c>
       <c r="B61">
-        <v>0.4744389027431422</v>
+        <v>0.5390070921985816</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -5279,7 +5279,7 @@
         <v>36</v>
       </c>
       <c r="B62">
-        <v>0.4644808743169399</v>
+        <v>0.5220966084275437</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5287,7 +5287,7 @@
         <v>420</v>
       </c>
       <c r="B63">
-        <v>0.4813895781637717</v>
+        <v>0.5606936416184971</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5295,7 +5295,7 @@
         <v>421</v>
       </c>
       <c r="B64">
-        <v>0.479328165374677</v>
+        <v>0.5672333848531684</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5303,7 +5303,7 @@
         <v>422</v>
       </c>
       <c r="B65">
-        <v>0.5158562367864693</v>
+        <v>0.5929526123936817</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -5311,7 +5311,7 @@
         <v>423</v>
       </c>
       <c r="B66">
-        <v>0.4736842105263158</v>
+        <v>0.5869565217391305</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -5319,7 +5319,7 @@
         <v>424</v>
       </c>
       <c r="B67">
-        <v>0.4839816933638444</v>
+        <v>0.5858725761772853</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -5327,7 +5327,7 @@
         <v>425</v>
       </c>
       <c r="B68">
-        <v>0.4347699475829936</v>
+        <v>0.5231578947368422</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5335,7 +5335,7 @@
         <v>426</v>
       </c>
       <c r="B69">
-        <v>0.4839181286549707</v>
+        <v>0.5892857142857143</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -5343,7 +5343,7 @@
         <v>427</v>
       </c>
       <c r="B70">
-        <v>0.4518518518518518</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5351,7 +5351,7 @@
         <v>428</v>
       </c>
       <c r="B71">
-        <v>0.4831568816169394</v>
+        <v>0.5574136008918618</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -5359,7 +5359,7 @@
         <v>429</v>
       </c>
       <c r="B72">
-        <v>0.4832451499118166</v>
+        <v>0.5508130081300813</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -5367,7 +5367,7 @@
         <v>430</v>
       </c>
       <c r="B73">
-        <v>0.4797527047913447</v>
+        <v>0.5758028379387603</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -5375,7 +5375,7 @@
         <v>431</v>
       </c>
       <c r="B74">
-        <v>0.4407894736842105</v>
+        <v>0.5153846153846153</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -5383,7 +5383,7 @@
         <v>432</v>
       </c>
       <c r="B75">
-        <v>0.4797546012269939</v>
+        <v>0.5561959654178674</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -5391,7 +5391,7 @@
         <v>433</v>
       </c>
       <c r="B76">
-        <v>0.4592074592074592</v>
+        <v>0.5171503957783641</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -5399,7 +5399,7 @@
         <v>434</v>
       </c>
       <c r="B77">
-        <v>0.4775280898876405</v>
+        <v>0.5466377440347071</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5407,7 +5407,7 @@
         <v>435</v>
       </c>
       <c r="B78">
-        <v>0.5361271676300579</v>
+        <v>0.6368330464716007</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -5415,7 +5415,7 @@
         <v>436</v>
       </c>
       <c r="B79">
-        <v>0.4675652906486942</v>
+        <v>0.5698151950718686</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -5423,7 +5423,7 @@
         <v>437</v>
       </c>
       <c r="B80">
-        <v>0.4977293369663942</v>
+        <v>0.5794491525423728</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -5431,7 +5431,7 @@
         <v>438</v>
       </c>
       <c r="B81">
-        <v>0.5016181229773463</v>
+        <v>0.5996131528046421</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -5439,7 +5439,7 @@
         <v>439</v>
       </c>
       <c r="B82">
-        <v>0.4946236559139785</v>
+        <v>0.5843920145190563</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -5447,7 +5447,7 @@
         <v>440</v>
       </c>
       <c r="B83">
-        <v>0.5354477611940298</v>
+        <v>0.6377777777777778</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -5455,7 +5455,7 @@
         <v>441</v>
       </c>
       <c r="B84">
-        <v>0.4798099762470309</v>
+        <v>0.5740740740740741</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -5463,7 +5463,7 @@
         <v>442</v>
       </c>
       <c r="B85">
-        <v>0.4127218934911243</v>
+        <v>0.4696969696969697</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -5471,7 +5471,7 @@
         <v>443</v>
       </c>
       <c r="B86">
-        <v>0.4941022280471822</v>
+        <v>0.5773353751914242</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -5479,7 +5479,7 @@
         <v>444</v>
       </c>
       <c r="B87">
-        <v>0.4821186057039384</v>
+        <v>0.5493472584856397</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -5487,7 +5487,7 @@
         <v>445</v>
       </c>
       <c r="B88">
-        <v>0.5045537340619308</v>
+        <v>0.5794979079497908</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -5495,7 +5495,7 @@
         <v>446</v>
       </c>
       <c r="B89">
-        <v>0.5061728395061729</v>
+        <v>0.5858369098712446</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -5503,7 +5503,7 @@
         <v>447</v>
       </c>
       <c r="B90">
-        <v>0.4565217391304348</v>
+        <v>0.5196850393700787</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -5511,7 +5511,7 @@
         <v>448</v>
       </c>
       <c r="B91">
-        <v>0.5258855585831063</v>
+        <v>0.6205787781350482</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -5519,7 +5519,7 @@
         <v>449</v>
       </c>
       <c r="B92">
-        <v>0.5309734513274337</v>
+        <v>0.6033613445378151</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -5527,7 +5527,7 @@
         <v>450</v>
       </c>
       <c r="B93">
-        <v>0.4912280701754386</v>
+        <v>0.5828571428571429</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -5535,7 +5535,7 @@
         <v>451</v>
       </c>
       <c r="B94">
-        <v>0.4339706536238328</v>
+        <v>0.4917948717948718</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -5543,7 +5543,7 @@
         <v>452</v>
       </c>
       <c r="B95">
-        <v>0.4564950980392157</v>
+        <v>0.5443873807776962</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -5551,7 +5551,7 @@
         <v>453</v>
       </c>
       <c r="B96">
-        <v>0.4980595084087969</v>
+        <v>0.5859969558599696</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -5559,7 +5559,7 @@
         <v>454</v>
       </c>
       <c r="B97">
-        <v>0.5062344139650873</v>
+        <v>0.5953079178885631</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -5567,7 +5567,7 @@
         <v>455</v>
       </c>
       <c r="B98">
-        <v>0.5062344139650873</v>
+        <v>0.5953079178885631</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -5575,7 +5575,7 @@
         <v>456</v>
       </c>
       <c r="B99">
-        <v>0.5115131578947368</v>
+        <v>0.5769944341372912</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -5583,7 +5583,7 @@
         <v>457</v>
       </c>
       <c r="B100">
-        <v>0.4592592592592593</v>
+        <v>0.5520504731861199</v>
       </c>
     </row>
   </sheetData>
@@ -5612,7 +5612,7 @@
         <v>458</v>
       </c>
       <c r="B2">
-        <v>0.4898477157360406</v>
+        <v>0.5520231213872833</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5620,7 +5620,7 @@
         <v>459</v>
       </c>
       <c r="B3">
-        <v>0.4839572192513369</v>
+        <v>0.5934426229508196</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5628,7 +5628,7 @@
         <v>460</v>
       </c>
       <c r="B4">
-        <v>0.489051094890511</v>
+        <v>0.5495867768595041</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5636,7 +5636,7 @@
         <v>461</v>
       </c>
       <c r="B5">
-        <v>0.4745762711864407</v>
+        <v>0.5490196078431373</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5644,7 +5644,7 @@
         <v>462</v>
       </c>
       <c r="B6">
-        <v>0.4805115712545676</v>
+        <v>0.5633500357909806</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5652,7 +5652,7 @@
         <v>463</v>
       </c>
       <c r="B7">
-        <v>0.4625445897740785</v>
+        <v>0.5413953488372093</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5660,7 +5660,7 @@
         <v>464</v>
       </c>
       <c r="B8">
-        <v>0.4509056244041945</v>
+        <v>0.5455594002306805</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5668,7 +5668,7 @@
         <v>465</v>
       </c>
       <c r="B9">
-        <v>0.4890965732087227</v>
+        <v>0.564748201438849</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5676,7 +5676,7 @@
         <v>466</v>
       </c>
       <c r="B10">
-        <v>0.4024943310657597</v>
+        <v>0.4689564068692206</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5684,7 +5684,7 @@
         <v>467</v>
       </c>
       <c r="B11">
-        <v>0.5162790697674419</v>
+        <v>0.6021798365122616</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5692,7 +5692,7 @@
         <v>468</v>
       </c>
       <c r="B12">
-        <v>0.5114754098360655</v>
+        <v>0.5897920604914934</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5700,7 +5700,7 @@
         <v>469</v>
       </c>
       <c r="B13">
-        <v>0.5060658578856152</v>
+        <v>0.605427974947808</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5708,7 +5708,7 @@
         <v>470</v>
       </c>
       <c r="B14">
-        <v>0.4105642256902761</v>
+        <v>0.527047913446677</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5716,7 +5716,7 @@
         <v>471</v>
       </c>
       <c r="B15">
-        <v>0.4702702702702703</v>
+        <v>0.5615550755939525</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5724,7 +5724,7 @@
         <v>472</v>
       </c>
       <c r="B16">
-        <v>0.4746543778801843</v>
+        <v>0.5819209039548022</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5732,7 +5732,7 @@
         <v>473</v>
       </c>
       <c r="B17">
-        <v>0.4919564089257914</v>
+        <v>0.5828712261244609</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -5740,7 +5740,7 @@
         <v>474</v>
       </c>
       <c r="B18">
-        <v>0.3461538461538461</v>
+        <v>0.4029850746268657</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5748,7 +5748,7 @@
         <v>475</v>
       </c>
       <c r="B19">
-        <v>0.5006418485237484</v>
+        <v>0.5756676557863502</v>
       </c>
     </row>
   </sheetData>
@@ -5801,25 +5801,25 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>0.4806027821189309</v>
+        <v>0.5537066413504576</v>
       </c>
       <c r="D2">
-        <v>0.0447953097810643</v>
+        <v>0.04543171633570749</v>
       </c>
       <c r="E2">
-        <v>0.3931203931203931</v>
+        <v>0.4678362573099415</v>
       </c>
       <c r="F2">
-        <v>0.4529128862814653</v>
+        <v>0.5222665925289389</v>
       </c>
       <c r="G2">
-        <v>0.4744318181818182</v>
+        <v>0.5461847389558233</v>
       </c>
       <c r="H2">
-        <v>0.5079393083980239</v>
+        <v>0.5891412981445137</v>
       </c>
       <c r="I2">
-        <v>0.5608974358974359</v>
+        <v>0.6225402504472272</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -5830,25 +5830,25 @@
         <v>113</v>
       </c>
       <c r="C3">
-        <v>0.4847874237125769</v>
+        <v>0.5641475705197292</v>
       </c>
       <c r="D3">
-        <v>0.03986116952942371</v>
+        <v>0.04734096807539965</v>
       </c>
       <c r="E3">
-        <v>0.4070021881838075</v>
+        <v>0.4698162729658792</v>
       </c>
       <c r="F3">
-        <v>0.4606824925816024</v>
+        <v>0.5342465753424658</v>
       </c>
       <c r="G3">
-        <v>0.4784172661870504</v>
+        <v>0.559322033898305</v>
       </c>
       <c r="H3">
-        <v>0.510351966873706</v>
+        <v>0.5894428152492669</v>
       </c>
       <c r="I3">
-        <v>0.6702127659574468</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5859,25 +5859,25 @@
         <v>152</v>
       </c>
       <c r="C4">
-        <v>0.4783164053584509</v>
+        <v>0.5612005571449178</v>
       </c>
       <c r="D4">
-        <v>0.03233080807523336</v>
+        <v>0.05155526408206184</v>
       </c>
       <c r="E4">
-        <v>0.38</v>
+        <v>0.4473684210526316</v>
       </c>
       <c r="F4">
-        <v>0.4596767064986086</v>
+        <v>0.5358351965745919</v>
       </c>
       <c r="G4">
-        <v>0.4776594733339671</v>
+        <v>0.5583820899278312</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.583667323954506</v>
       </c>
       <c r="I4">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -5888,25 +5888,25 @@
         <v>74</v>
       </c>
       <c r="C5">
-        <v>0.4764252857849724</v>
+        <v>0.5585400828185515</v>
       </c>
       <c r="D5">
-        <v>0.03611408955883882</v>
+        <v>0.03816459313230278</v>
       </c>
       <c r="E5">
-        <v>0.4125</v>
+        <v>0.4926108374384237</v>
       </c>
       <c r="F5">
-        <v>0.4522481987806009</v>
+        <v>0.5295607627359833</v>
       </c>
       <c r="G5">
-        <v>0.4794081427078024</v>
+        <v>0.5607816034179443</v>
       </c>
       <c r="H5">
-        <v>0.4982671205160553</v>
+        <v>0.5821139067270239</v>
       </c>
       <c r="I5">
-        <v>0.5769230769230769</v>
+        <v>0.6578947368421053</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5917,25 +5917,25 @@
         <v>99</v>
       </c>
       <c r="C6">
-        <v>0.4811347084593117</v>
+        <v>0.5657496254289831</v>
       </c>
       <c r="D6">
-        <v>0.03438132014714517</v>
+        <v>0.04038283184447704</v>
       </c>
       <c r="E6">
-        <v>0.3962264150943396</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="F6">
-        <v>0.458999333999334</v>
+        <v>0.5384522013560145</v>
       </c>
       <c r="G6">
-        <v>0.4831568816169394</v>
+        <v>0.5698151950718686</v>
       </c>
       <c r="H6">
-        <v>0.5042677657795434</v>
+        <v>0.5924557364839703</v>
       </c>
       <c r="I6">
-        <v>0.6028119507908611</v>
+        <v>0.692929292929293</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5946,25 +5946,25 @@
         <v>18</v>
       </c>
       <c r="C7">
-        <v>0.4695025725391606</v>
+        <v>0.5531960690940197</v>
       </c>
       <c r="D7">
-        <v>0.04331584855749605</v>
+        <v>0.04921535816901217</v>
       </c>
       <c r="E7">
-        <v>0.3461538461538461</v>
+        <v>0.4029850746268657</v>
       </c>
       <c r="F7">
-        <v>0.4644760098981264</v>
+        <v>0.5464244521337946</v>
       </c>
       <c r="G7">
-        <v>0.4822343952529523</v>
+        <v>0.5624525556924665</v>
       </c>
       <c r="H7">
-        <v>0.4914292356283537</v>
+        <v>0.5826336455820462</v>
       </c>
       <c r="I7">
-        <v>0.5162790697674419</v>
+        <v>0.605427974947808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>